<commit_message>
Update class codes 2023, fix script
</commit_message>
<xml_diff>
--- a/data/source/reference/chicago_crime_classifications.xlsx
+++ b/data/source/reference/chicago_crime_classifications.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Jarvis/R/safetytracker_chicago/data/source/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99141FBD-E29C-8840-A280-53D85645D742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616CA362-A341-714C-B3F0-9BE8283DFF71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40700" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{2C83FEE3-5951-9549-9A6B-752E62C644CA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19320" xr2:uid="{2C83FEE3-5951-9549-9A6B-752E62C644CA}"/>
   </bookViews>
   <sheets>
     <sheet name="chicago_codes" sheetId="5" r:id="rId1"/>
@@ -42,7 +42,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{D0C93D55-09B4-D944-A06C-4AEA7DB9179C}" name="chicago_crime_classifications" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Volumes/Jarvis/R/safetytracker_chicago/data/source/reference/chicago_crime_classifications.csv" tab="0" comma="1">
+    <textPr sourceFile="/Volumes/Jarvis/R/safetytracker_chicago/data/source/reference/chicago_crime_classifications.csv" tab="0" comma="1">
       <textFields count="6">
         <textField type="text"/>
         <textField type="text"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2460" uniqueCount="883">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2464" uniqueCount="884">
   <si>
     <t>HOMICIDE FIRST DEGREE MURDER</t>
   </si>
@@ -2706,19 +2706,28 @@
   </si>
   <si>
     <t>Property</t>
+  </si>
+  <si>
+    <t>TIRE DEFLATION DEVICE DEPLOYMENT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF080808"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2741,9 +2750,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3062,10 +3072,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBCB7161-5171-2545-980C-338858D2F3B6}">
-  <dimension ref="A1:F410"/>
+  <dimension ref="A1:F411"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A267" workbookViewId="0">
-      <selection activeCell="B298" sqref="B298"/>
+    <sheetView tabSelected="1" topLeftCell="A384" workbookViewId="0">
+      <selection activeCell="F394" sqref="F394"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11278,6 +11288,26 @@
         <v>398</v>
       </c>
     </row>
+    <row r="411" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A411" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="B411" s="1">
+        <v>24</v>
+      </c>
+      <c r="C411" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="D411" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="E411" s="1">
+        <v>2896</v>
+      </c>
+      <c r="F411" s="2" t="s">
+        <v>883</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F410" xr:uid="{BBCB7161-5171-2545-980C-338858D2F3B6}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F410">

</xml_diff>